<commit_message>
Start Add Dish Portrait
</commit_message>
<xml_diff>
--- a/Dish Excel Document.xlsx
+++ b/Dish Excel Document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\A2\Unity\Cooking_Clicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02138ED9-BCAB-4795-B995-F0E16BC5ADE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB52AFC-C399-4842-93D4-AC262DE1FBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-555" windowWidth="38640" windowHeight="21120" xr2:uid="{FBB31979-A78A-4D7A-9C52-45433E30BBAE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Tomato</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Plancha-seared veal and bean salad</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -242,13 +245,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -564,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19068C32-9D69-4585-A414-993633583C8F}">
-  <dimension ref="B2:AA34"/>
+  <dimension ref="A2:AA34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,7 +577,7 @@
     <col min="2" max="2" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +651,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
@@ -686,7 +688,7 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
@@ -723,7 +725,7 @@
       </c>
       <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -760,7 +762,7 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
@@ -799,7 +801,7 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -834,7 +836,7 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -873,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -912,7 +914,7 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
@@ -949,7 +951,7 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
@@ -986,7 +988,7 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1023,7 +1025,7 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1056,7 +1058,10 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1091,7 +1096,7 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1126,7 +1131,7 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1199,7 +1204,7 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="3"/>
@@ -1236,7 +1241,7 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="3"/>
@@ -1252,9 +1257,9 @@
         <v>1</v>
       </c>
       <c r="M19" s="3"/>
-      <c r="N19" s="6"/>
+      <c r="N19" s="5"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="6"/>
+      <c r="P19" s="5"/>
       <c r="Q19" s="4">
         <v>2</v>
       </c>
@@ -1271,7 +1276,7 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="3"/>
@@ -1310,7 +1315,7 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="3"/>
@@ -1347,7 +1352,7 @@
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="3"/>
@@ -1384,7 +1389,7 @@
       <c r="AA22" s="2"/>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="3"/>

</xml_diff>